<commit_message>
Range anxiety shadow costs updated to reflect IIJA, psgr-LDV shareweights updated to match other states' values
</commit_message>
<xml_diff>
--- a/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
+++ b/InputData/trans/BRAaCTSC/BAU Rng Anxiety and Charge Time Shadow Costs.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us-analysis\InputData\trans\BRAaCTSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BRAaCTSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA3E91-76B2-4E00-B280-A24BBC976430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02F20B-346B-4E17-A776-81D370EAD24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="4" r:id="rId2"/>
-    <sheet name="BRAaCTSC" sheetId="3" r:id="rId3"/>
+    <sheet name="EV charger assumptions" sheetId="5" r:id="rId3"/>
+    <sheet name="BRAaCTSC" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="income">Calculations!$B$10</definedName>
     <definedName name="Range_EV">Calculations!$B$9</definedName>
     <definedName name="range_ICE">Calculations!$B$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Source:</t>
   </si>
@@ -152,9 +153,6 @@
     <t>https://www.nrel.gov/docs/fy13osti/55639.pdf</t>
   </si>
   <si>
-    <t>EVSE ports:</t>
-  </si>
-  <si>
     <t>Number of gas pumps</t>
   </si>
   <si>
@@ -233,12 +231,6 @@
     <t>Calculations</t>
   </si>
   <si>
-    <t>Year 2020</t>
-  </si>
-  <si>
-    <t>Year 2050</t>
-  </si>
-  <si>
     <t xml:space="preserve">250 miles and is forecated to continue improving. Therefore, we start with today's median range, and assume </t>
   </si>
   <si>
@@ -248,7 +240,31 @@
     <t>EV charging ports and gas pumps. We also assume this value will decline to 0 by 2050 as more EV chargers come online.</t>
   </si>
   <si>
-    <t>Year 2030</t>
+    <t xml:space="preserve">*2020 median range taken from historical data. 2030 and 2050 are estimated, with the 2050 </t>
+  </si>
+  <si>
+    <t>range roughly corresponding to today's maximum range</t>
+  </si>
+  <si>
+    <t>We assume EV charger additions based on investments in the Infrastructure Investment and Jobs Act</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total government funding: </t>
+  </si>
+  <si>
+    <t>($7.5 billion between 2022 and 2026), assuming 80% of the costs are paid for by the government.</t>
+  </si>
+  <si>
+    <t>Total government + private funding:</t>
+  </si>
+  <si>
+    <t>Average weighted charger cost (see trans/EVCC):</t>
+  </si>
+  <si>
+    <t>Chargers added by 2026:</t>
+  </si>
+  <si>
+    <t>2020 EVSE ports:</t>
   </si>
 </sst>
 </file>
@@ -258,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +284,22 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -298,10 +330,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -315,8 +348,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,11 +458,47 @@
             </c:spPr>
             <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.8828958880139982E-2"/>
+                  <c:y val="-0.13703885898644008"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Calculations!$A$16:$A$19</c:f>
+              <c:f>Calculations!$A$17:$A$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -444,7 +519,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Calculations!$B$16:$B$19</c:f>
+              <c:f>Calculations!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1225,7 +1300,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>292100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1521,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,12 +1667,12 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -1607,22 +1682,22 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
@@ -1632,17 +1707,17 @@
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -1657,27 +1732,27 @@
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1687,12 +1762,12 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="9" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1715,42 +1790,42 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1762,21 +1837,24 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B38" r:id="rId1" xr:uid="{14EF0A86-0973-41E2-9D23-51C96C77958E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341A17B3-AFD9-42DA-AB68-E46FC6CF1D40}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1815,19 +1893,19 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
+      <c r="B7">
+        <v>2020</v>
+      </c>
+      <c r="C7">
+        <v>2030</v>
+      </c>
+      <c r="D7">
+        <v>2050</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>4.12</v>
@@ -1847,10 +1925,10 @@
       <c r="B9">
         <v>2.59</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>4.12</v>
       </c>
     </row>
@@ -1861,155 +1939,210 @@
       <c r="B10">
         <v>68.703000000000003</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <f>income</f>
         <v>68.703000000000003</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <f>B10</f>
         <v>68.703000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="6">
-        <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)</f>
-        <v>8.7776895901028578</v>
-      </c>
-      <c r="C13" s="6">
-        <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)</f>
-        <v>5.8013729917508945</v>
-      </c>
-      <c r="D13" s="6">
-        <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)</f>
+      <c r="B14" s="6">
+        <f>($B$4/$B$2*B9*(1-B8/B9)+$B$5/$B$2*B9^2*(1-B8^2/B9^2))*LN(income)*About!$B$53</f>
+        <v>7.8828464065137096</v>
+      </c>
+      <c r="C14" s="6">
+        <f>($B$4/$B$2*C9*(1-C8/C9)+$B$5/$B$2*C9^2*(1-C8^2/C9^2))*LN(income)*About!$B$53</f>
+        <v>5.2099509525186276</v>
+      </c>
+      <c r="D14" s="6">
+        <f>($B$4/$B$2*D9*(1-D8/D9)+$B$5/$B$2*D9^2*(1-D8^2/D9^2))*LN(income)*About!$B$53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>7500</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>0.05</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>1750</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>0.1</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>1</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24">
+        <v>120045</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B23">
-        <v>120045</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B25">
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>2020</v>
+      </c>
+      <c r="C27">
+        <v>2027</v>
+      </c>
+      <c r="D27">
+        <v>2030</v>
+      </c>
+      <c r="E27">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B24">
-        <v>1200000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B28">
+        <f>B24/B25</f>
+        <v>0.1000375</v>
+      </c>
+      <c r="C28">
+        <f>(B24+'EV charger assumptions'!B9)/Calculations!B25</f>
+        <v>0.41965865943214825</v>
+      </c>
+      <c r="D28">
+        <f>(E28-C28)/(E27-C27)*3+C28</f>
+        <v>0.495355356027955</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B25">
-        <f>B23/B24</f>
-        <v>0.1000375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26">
-        <f>B18</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B29">
+        <f>B19*About!$B$53</f>
+        <v>898.05481563188175</v>
+      </c>
+      <c r="C29">
+        <f>-667.1*LN(C28)-241.23</f>
+        <v>338.02201174921117</v>
+      </c>
+      <c r="D29">
+        <f>-667.1*LN(D28)-241.23</f>
+        <v>227.39432995486422</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>2020</v>
       </c>
-      <c r="B33">
-        <f>B13*1000+B26</f>
-        <v>9777.6895901028583</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B36">
+        <f>B14*1000+B29</f>
+        <v>8780.9012221455905</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2027</v>
+      </c>
+      <c r="B37" cm="1">
+        <f t="array" ref="B37">TREND(B14:C14,B7:C7,C27)*1000+C29</f>
+        <v>6349.8416004663277</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>2030</v>
       </c>
-      <c r="B34">
-        <f>C13*1000+B26</f>
-        <v>6801.3729917508945</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B38">
+        <f>C14*1000+D29</f>
+        <v>5437.3452824734923</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>2050</v>
       </c>
-      <c r="B35">
-        <f>D13*1000+B26</f>
-        <v>1000</v>
+      <c r="B39">
+        <f>D14*1000+E29</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2020,14 +2153,77 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D98A39-3A78-451F-9516-0CF8624C92E2}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>7500000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5">
+        <f>B4/0.8</f>
+        <v>9375000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>24443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B5/B7</f>
+        <v>383545.39131857792</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,128 +2334,128 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" cm="1">
-        <f t="array" ref="B2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!B1)</f>
-        <v>9777.6895901027601</v>
+        <f t="array" ref="B2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!B1)</f>
+        <v>8780.9012221456505</v>
       </c>
       <c r="C2" s="3" cm="1">
-        <f t="array" ref="C2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!C1)</f>
-        <v>9480.0579302676488</v>
+        <f t="array" ref="C2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!C1)</f>
+        <v>8433.6069904771866</v>
       </c>
       <c r="D2" s="3" cm="1">
-        <f t="array" ref="D2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!D1)</f>
-        <v>9182.426270432421</v>
+        <f t="array" ref="D2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!D1)</f>
+        <v>8086.3127588086063</v>
       </c>
       <c r="E2" s="3" cm="1">
-        <f t="array" ref="E2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!E1)</f>
-        <v>8884.7946105971932</v>
+        <f t="array" ref="E2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!E1)</f>
+        <v>7739.0185271401424</v>
       </c>
       <c r="F2" s="3" cm="1">
-        <f t="array" ref="F2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!F1)</f>
-        <v>8587.1629507620819</v>
+        <f t="array" ref="F2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!F1)</f>
+        <v>7391.7242954716785</v>
       </c>
       <c r="G2" s="3" cm="1">
-        <f t="array" ref="G2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!G1)</f>
-        <v>8289.5312909268541</v>
+        <f t="array" ref="G2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!G1)</f>
+        <v>7044.4300638032146</v>
       </c>
       <c r="H2" s="3" cm="1">
-        <f t="array" ref="H2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!H1)</f>
-        <v>7991.8996310916264</v>
+        <f t="array" ref="H2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!H1)</f>
+        <v>6697.1358321347507</v>
       </c>
       <c r="I2" s="3" cm="1">
-        <f t="array" ref="I2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!I1)</f>
-        <v>7694.2679712563986</v>
+        <f t="array" ref="I2">TREND(Calculations!$B$36:$B$37,Calculations!$A$36:$A$37,BRAaCTSC!I1)</f>
+        <v>6349.8416004662868</v>
       </c>
       <c r="J2" s="3" cm="1">
-        <f t="array" ref="J2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!J1)</f>
-        <v>7396.6363114212872</v>
+        <f t="array" ref="J2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!J1)</f>
+        <v>6045.6761611354304</v>
       </c>
       <c r="K2" s="3" cm="1">
-        <f t="array" ref="K2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!K1)</f>
-        <v>7099.0046515860595</v>
+        <f t="array" ref="K2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!K1)</f>
+        <v>5741.5107218045741</v>
       </c>
       <c r="L2" s="3" cm="1">
-        <f t="array" ref="L2">TREND(Calculations!$B$33:$B$34,Calculations!$A$33:$A$34,BRAaCTSC!L1)</f>
-        <v>6801.3729917508317</v>
+        <f t="array" ref="L2">TREND(Calculations!$B$37:$B$38,Calculations!$A$37:$A$38,BRAaCTSC!L1)</f>
+        <v>5437.3452824736014</v>
       </c>
       <c r="M2" s="3" cm="1">
-        <f t="array" ref="M2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!M1)</f>
-        <v>6511.3043421633774</v>
+        <f t="array" ref="M2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!M1)</f>
+        <v>5165.4780183498515</v>
       </c>
       <c r="N2" s="3" cm="1">
-        <f t="array" ref="N2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!N1)</f>
-        <v>6221.2356925758068</v>
+        <f t="array" ref="N2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!N1)</f>
+        <v>4893.610754226218</v>
       </c>
       <c r="O2" s="3" cm="1">
-        <f t="array" ref="O2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!O1)</f>
-        <v>5931.1670429883525</v>
+        <f t="array" ref="O2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!O1)</f>
+        <v>4621.7434901024681</v>
       </c>
       <c r="P2" s="3" cm="1">
-        <f t="array" ref="P2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!P1)</f>
-        <v>5641.0983934007818</v>
+        <f t="array" ref="P2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!P1)</f>
+        <v>4349.8762259788346</v>
       </c>
       <c r="Q2" s="3" cm="1">
-        <f t="array" ref="Q2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Q1)</f>
-        <v>5351.0297438132111</v>
+        <f t="array" ref="Q2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Q1)</f>
+        <v>4078.0089618552011</v>
       </c>
       <c r="R2" s="3" cm="1">
-        <f t="array" ref="R2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!R1)</f>
-        <v>5060.9610942256404</v>
+        <f t="array" ref="R2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!R1)</f>
+        <v>3806.1416977314511</v>
       </c>
       <c r="S2" s="3" cm="1">
-        <f t="array" ref="S2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!S1)</f>
-        <v>4770.8924446381861</v>
+        <f t="array" ref="S2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!S1)</f>
+        <v>3534.2744336078176</v>
       </c>
       <c r="T2" s="3" cm="1">
-        <f t="array" ref="T2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!T1)</f>
-        <v>4480.8237950506154</v>
+        <f t="array" ref="T2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!T1)</f>
+        <v>3262.4071694841841</v>
       </c>
       <c r="U2" s="3" cm="1">
-        <f t="array" ref="U2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!U1)</f>
-        <v>4190.7551454630448</v>
+        <f t="array" ref="U2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!U1)</f>
+        <v>2990.5399053604342</v>
       </c>
       <c r="V2" s="3" cm="1">
-        <f t="array" ref="V2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!V1)</f>
-        <v>3900.6864958754741</v>
+        <f t="array" ref="V2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!V1)</f>
+        <v>2718.6726412368007</v>
       </c>
       <c r="W2" s="3" cm="1">
-        <f t="array" ref="W2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!W1)</f>
-        <v>3610.6178462879034</v>
+        <f t="array" ref="W2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!W1)</f>
+        <v>2446.8053771130508</v>
       </c>
       <c r="X2" s="3" cm="1">
-        <f t="array" ref="X2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!X1)</f>
-        <v>3320.5491967004491</v>
+        <f t="array" ref="X2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!X1)</f>
+        <v>2174.9381129894173</v>
       </c>
       <c r="Y2" s="3" cm="1">
-        <f t="array" ref="Y2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Y1)</f>
-        <v>3030.4805471128784</v>
+        <f t="array" ref="Y2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Y1)</f>
+        <v>1903.0708488657838</v>
       </c>
       <c r="Z2" s="3" cm="1">
-        <f t="array" ref="Z2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!Z1)</f>
-        <v>2740.4118975253077</v>
+        <f t="array" ref="Z2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!Z1)</f>
+        <v>1631.2035847420339</v>
       </c>
       <c r="AA2" s="3" cm="1">
-        <f t="array" ref="AA2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AA1)</f>
-        <v>2450.343247937737</v>
+        <f t="array" ref="AA2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AA1)</f>
+        <v>1359.3363206184004</v>
       </c>
       <c r="AB2" s="3" cm="1">
-        <f t="array" ref="AB2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AB1)</f>
-        <v>2160.2745983502828</v>
+        <f t="array" ref="AB2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AB1)</f>
+        <v>1087.4690564947668</v>
       </c>
       <c r="AC2" s="3" cm="1">
-        <f t="array" ref="AC2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AC1)</f>
-        <v>1870.2059487627121</v>
+        <f t="array" ref="AC2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AC1)</f>
+        <v>815.60179237101693</v>
       </c>
       <c r="AD2" s="3" cm="1">
-        <f t="array" ref="AD2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AD1)</f>
-        <v>1580.1372991751414</v>
+        <f t="array" ref="AD2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AD1)</f>
+        <v>543.73452824738342</v>
       </c>
       <c r="AE2" s="3" cm="1">
-        <f t="array" ref="AE2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AE1)</f>
-        <v>1290.0686495875707</v>
+        <f t="array" ref="AE2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AE1)</f>
+        <v>271.86726412374992</v>
       </c>
       <c r="AF2" s="3" cm="1">
-        <f t="array" ref="AF2">TREND(Calculations!$B$34:$B$35,Calculations!$A$34:$A$35,BRAaCTSC!AF1)</f>
-        <v>1000</v>
+        <f t="array" ref="AF2">TREND(Calculations!$B$38:$B$39,Calculations!$A$38:$A$39,BRAaCTSC!AF1)</f>
+        <v>0</v>
       </c>
       <c r="AG2" s="3"/>
     </row>

</xml_diff>